<commit_message>
Continued slides for W4.
</commit_message>
<xml_diff>
--- a/Extras/Names_list.xlsx
+++ b/Extras/Names_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/matthieu_demari_sutd_edu_sg/Documents/Teaching folder for web/9. DL @ SUTD 2021-ongoing/Teaching Materials/1. Lectures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/matthieu_demari_sutd_edu_sg/Documents/Teaching folder for web/9. DL @ SUTD 2021-ongoing/Teaching Materials/1. Lectures/Extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="56" documentId="11_F25DC773A252ABDACC10480EB1D941EE5BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8609FA23-6578-43B2-AF05-8AE5216620AC}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1185" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Releasing W4S1 materials, minor typos corrected.
</commit_message>
<xml_diff>
--- a/Extras/Names_list.xlsx
+++ b/Extras/Names_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/matthieu_demari_sutd_edu_sg/Documents/Teaching folder for web/9. DL @ SUTD 2021-ongoing/Teaching Materials/1. Lectures/Extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="11_F25DC773A252ABDACC10480EB1D941EE5BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46DB0E33-4B95-40BB-BC02-CF5FF0430492}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="11_F25DC773A252ABDACC10480EB1D941EE5BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D10EA2A-F820-49F6-AB4D-2D4691C09DCA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,20 +190,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -215,14 +219,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -504,7 +510,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Done with W4S2 and W4S3 materials.
</commit_message>
<xml_diff>
--- a/Extras/Names_list.xlsx
+++ b/Extras/Names_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/matthieu_demari_sutd_edu_sg/Documents/Teaching folder for web/9. DL @ SUTD 2021-ongoing/Teaching Materials/1. Lectures/Extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="11_F25DC773A252ABDACC10480EB1D941EE5BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D10EA2A-F820-49F6-AB4D-2D4691C09DCA}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="11_F25DC773A252ABDACC10480EB1D941EE5BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3F246F3-21E9-49E0-82AE-8C507F06112A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Family name</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>Jian</t>
+  </si>
+  <si>
+    <t>Quoc V.</t>
+  </si>
+  <si>
+    <t>Le</t>
   </si>
 </sst>
 </file>
@@ -507,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,6 +876,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Move adversarial ML to W5.
</commit_message>
<xml_diff>
--- a/Extras/Names_list.xlsx
+++ b/Extras/Names_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/matthieu_demari_sutd_edu_sg/Documents/Teaching folder for web/9. DL @ SUTD 2021-ongoing/Teaching Materials/1. Lectures/Extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="11_F25DC773A252ABDACC10480EB1D941EE5BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3F246F3-21E9-49E0-82AE-8C507F06112A}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="11_F25DC773A252ABDACC10480EB1D941EE5BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{270DFDE3-A896-4B00-9275-BD0B8F03F0FA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>Family name</t>
   </si>
@@ -181,6 +181,42 @@
   </si>
   <si>
     <t>Le</t>
+  </si>
+  <si>
+    <t>Goofellow</t>
+  </si>
+  <si>
+    <t>Ian</t>
+  </si>
+  <si>
+    <t>Kurakin</t>
+  </si>
+  <si>
+    <t>Alexei</t>
+  </si>
+  <si>
+    <t>Samy</t>
+  </si>
+  <si>
+    <t>Madry</t>
+  </si>
+  <si>
+    <t>Aleksander</t>
+  </si>
+  <si>
+    <t>Papernot</t>
+  </si>
+  <si>
+    <t>Nicolas</t>
+  </si>
+  <si>
+    <t>Carlini</t>
+  </si>
+  <si>
+    <t>Nicholas</t>
+  </si>
+  <si>
+    <t>Wagner</t>
   </si>
 </sst>
 </file>
@@ -513,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,6 +926,104 @@
         <v>3</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Added GRU materials to W6.
</commit_message>
<xml_diff>
--- a/Extras/Names_list.xlsx
+++ b/Extras/Names_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/matthieu_demari_sutd_edu_sg/Documents/Teaching folder for web/9. DL @ SUTD 2021-ongoing/Teaching Materials/1. Lectures/Extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="11_F25DC773A252ABDACC10480EB1D941EE5BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{270DFDE3-A896-4B00-9275-BD0B8F03F0FA}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="11_F25DC773A252ABDACC10480EB1D941EE5BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8AA183A-BE7F-4FBD-932D-4645FC21FC2C}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
   <si>
     <t>Family name</t>
   </si>
@@ -217,6 +217,18 @@
   </si>
   <si>
     <t>Wagner</t>
+  </si>
+  <si>
+    <t>Cho</t>
+  </si>
+  <si>
+    <t>Kyunghyun</t>
+  </si>
+  <si>
+    <t>Bahdanau</t>
+  </si>
+  <si>
+    <t>Dzmitri</t>
   </si>
 </sst>
 </file>
@@ -549,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,6 +1036,34 @@
         <v>3</v>
       </c>
     </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36">
+        <v>6</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>